<commit_message>
added author, career, country, quotes and subject to database
</commit_message>
<xml_diff>
--- a/00_Raw_Assets/quotes_v1.xlsx.xlsx
+++ b/00_Raw_Assets/quotes_v1.xlsx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://masseyhighschoolnz-my.sharepoint.com/personal/pereiraj72020_masseyhigh_school_nz/Documents/00_2021 files/Databases/91902_Quotes_DB/91902_Quotes_DB/00_Raw_Assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="539" documentId="13_ncr:40009_{9D8BBAB9-FE52-49AE-80E4-CBD616388BAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{96DDB198-4D6F-4359-8A59-E21D9AAB6823}"/>
+  <xr:revisionPtr revIDLastSave="550" documentId="13_ncr:40009_{9D8BBAB9-FE52-49AE-80E4-CBD616388BAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D9A9B61-9588-4658-9AEA-7A51406CF358}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="4215" windowWidth="21600" windowHeight="11385" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="2" r:id="rId1"/>
@@ -2424,7 +2424,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C33" sqref="C33"/>
+      <selection pane="bottomLeft" activeCell="F1" sqref="F1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9015,7 +9015,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79286491-E79E-4E2C-9899-AE987FCF5128}">
   <dimension ref="A1:G103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -9201,6 +9203,9 @@
       <c r="F9">
         <v>47</v>
       </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -9221,6 +9226,9 @@
       <c r="F10">
         <v>12</v>
       </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -9298,6 +9306,9 @@
       <c r="F14">
         <v>86</v>
       </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -9312,6 +9323,12 @@
       <c r="E15">
         <v>56</v>
       </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -9326,6 +9343,12 @@
       <c r="E16">
         <v>29</v>
       </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
@@ -9343,6 +9366,9 @@
       <c r="F17">
         <v>62</v>
       </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
@@ -9400,6 +9426,9 @@
       <c r="F20">
         <v>33</v>
       </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
@@ -9440,6 +9469,9 @@
       <c r="F22">
         <v>70</v>
       </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
@@ -9454,6 +9486,12 @@
       <c r="E23">
         <v>40</v>
       </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
@@ -9494,6 +9532,9 @@
       <c r="F25">
         <v>74</v>
       </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
@@ -9508,6 +9549,12 @@
       <c r="E26">
         <v>43</v>
       </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
@@ -9545,6 +9592,9 @@
       <c r="F28">
         <v>71</v>
       </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
@@ -9579,6 +9629,12 @@
       <c r="E30">
         <v>44</v>
       </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
@@ -9593,6 +9649,12 @@
       <c r="E31">
         <v>61</v>
       </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
@@ -9630,6 +9692,9 @@
       <c r="F33">
         <v>44</v>
       </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
@@ -9644,6 +9709,12 @@
       <c r="E34">
         <v>33</v>
       </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
@@ -9664,6 +9735,9 @@
       <c r="F35">
         <v>38</v>
       </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
@@ -9681,6 +9755,9 @@
       <c r="F36">
         <v>47</v>
       </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
@@ -9718,6 +9795,12 @@
       <c r="E38">
         <v>71</v>
       </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
@@ -9755,6 +9838,9 @@
       <c r="F40">
         <v>52</v>
       </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
@@ -9769,6 +9855,12 @@
       <c r="E41">
         <v>47</v>
       </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
@@ -9846,6 +9938,9 @@
       <c r="F45">
         <v>56</v>
       </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46">
@@ -9860,6 +9955,12 @@
       <c r="E46">
         <v>54</v>
       </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47">
@@ -9874,6 +9975,12 @@
       <c r="E47">
         <v>56</v>
       </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48">
@@ -9894,6 +10001,9 @@
       <c r="F48">
         <v>89</v>
       </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49">
@@ -9911,6 +10021,9 @@
       <c r="F49">
         <v>47</v>
       </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50">
@@ -9928,6 +10041,9 @@
       <c r="F50">
         <v>39</v>
       </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51">
@@ -9942,6 +10058,12 @@
       <c r="E51">
         <v>56</v>
       </c>
+      <c r="F51">
+        <v>0</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52">
@@ -9959,6 +10081,9 @@
       <c r="F52">
         <v>56</v>
       </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53">
@@ -9979,6 +10104,9 @@
       <c r="F53">
         <v>47</v>
       </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54">
@@ -10016,6 +10144,12 @@
       <c r="E55">
         <v>61</v>
       </c>
+      <c r="F55">
+        <v>0</v>
+      </c>
+      <c r="G55">
+        <v>0</v>
+      </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56">
@@ -10033,6 +10167,9 @@
       <c r="F56">
         <v>81</v>
       </c>
+      <c r="G56">
+        <v>0</v>
+      </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57">
@@ -10053,6 +10190,9 @@
       <c r="F57">
         <v>78</v>
       </c>
+      <c r="G57">
+        <v>0</v>
+      </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58">
@@ -10090,6 +10230,9 @@
       <c r="F59">
         <v>33</v>
       </c>
+      <c r="G59">
+        <v>0</v>
+      </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60">
@@ -10104,6 +10247,12 @@
       <c r="E60">
         <v>47</v>
       </c>
+      <c r="F60">
+        <v>0</v>
+      </c>
+      <c r="G60">
+        <v>0</v>
+      </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61">
@@ -10138,6 +10287,12 @@
       <c r="E62">
         <v>6</v>
       </c>
+      <c r="F62">
+        <v>0</v>
+      </c>
+      <c r="G62">
+        <v>0</v>
+      </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63">
@@ -10155,6 +10310,9 @@
       <c r="F63">
         <v>42</v>
       </c>
+      <c r="G63">
+        <v>0</v>
+      </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64">
@@ -10169,6 +10327,12 @@
       <c r="E64">
         <v>43</v>
       </c>
+      <c r="F64">
+        <v>0</v>
+      </c>
+      <c r="G64">
+        <v>0</v>
+      </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65">
@@ -10183,6 +10347,12 @@
       <c r="E65">
         <v>56</v>
       </c>
+      <c r="F65">
+        <v>0</v>
+      </c>
+      <c r="G65">
+        <v>0</v>
+      </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66">
@@ -10240,6 +10410,9 @@
       <c r="F68">
         <v>92</v>
       </c>
+      <c r="G68">
+        <v>0</v>
+      </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69">
@@ -10257,6 +10430,9 @@
       <c r="F69">
         <v>73</v>
       </c>
+      <c r="G69">
+        <v>0</v>
+      </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70">
@@ -10271,6 +10447,12 @@
       <c r="E70">
         <v>24</v>
       </c>
+      <c r="F70">
+        <v>0</v>
+      </c>
+      <c r="G70">
+        <v>0</v>
+      </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71">
@@ -10285,6 +10467,12 @@
       <c r="E71">
         <v>83</v>
       </c>
+      <c r="F71">
+        <v>0</v>
+      </c>
+      <c r="G71">
+        <v>0</v>
+      </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72">
@@ -10302,6 +10490,9 @@
       <c r="F72">
         <v>56</v>
       </c>
+      <c r="G72">
+        <v>0</v>
+      </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73">
@@ -10316,6 +10507,12 @@
       <c r="E73">
         <v>43</v>
       </c>
+      <c r="F73">
+        <v>0</v>
+      </c>
+      <c r="G73">
+        <v>0</v>
+      </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74">
@@ -10353,6 +10550,9 @@
       <c r="F75">
         <v>68</v>
       </c>
+      <c r="G75">
+        <v>0</v>
+      </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76">
@@ -10370,6 +10570,9 @@
       <c r="F76">
         <v>71</v>
       </c>
+      <c r="G76">
+        <v>0</v>
+      </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77">
@@ -10384,6 +10587,12 @@
       <c r="E77">
         <v>43</v>
       </c>
+      <c r="F77">
+        <v>0</v>
+      </c>
+      <c r="G77">
+        <v>0</v>
+      </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78">
@@ -10421,6 +10630,9 @@
       <c r="F79">
         <v>41</v>
       </c>
+      <c r="G79">
+        <v>0</v>
+      </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80">
@@ -10435,6 +10647,12 @@
       <c r="E80">
         <v>47</v>
       </c>
+      <c r="F80">
+        <v>0</v>
+      </c>
+      <c r="G80">
+        <v>0</v>
+      </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81">
@@ -10469,6 +10687,12 @@
       <c r="E82">
         <v>60</v>
       </c>
+      <c r="F82">
+        <v>0</v>
+      </c>
+      <c r="G82">
+        <v>0</v>
+      </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83">
@@ -10503,6 +10727,12 @@
       <c r="E84">
         <v>48</v>
       </c>
+      <c r="F84">
+        <v>0</v>
+      </c>
+      <c r="G84">
+        <v>0</v>
+      </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85">
@@ -10540,6 +10770,9 @@
       <c r="F86">
         <v>10</v>
       </c>
+      <c r="G86">
+        <v>0</v>
+      </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87">
@@ -10574,6 +10807,12 @@
       <c r="E88">
         <v>36</v>
       </c>
+      <c r="F88">
+        <v>0</v>
+      </c>
+      <c r="G88">
+        <v>0</v>
+      </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89">
@@ -10591,6 +10830,9 @@
       <c r="F89">
         <v>54</v>
       </c>
+      <c r="G89">
+        <v>0</v>
+      </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90">
@@ -10608,6 +10850,12 @@
       <c r="E90">
         <v>85</v>
       </c>
+      <c r="F90">
+        <v>0</v>
+      </c>
+      <c r="G90">
+        <v>0</v>
+      </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91">
@@ -10642,6 +10890,12 @@
       <c r="E92">
         <v>85</v>
       </c>
+      <c r="F92">
+        <v>0</v>
+      </c>
+      <c r="G92">
+        <v>0</v>
+      </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93">
@@ -10659,6 +10913,9 @@
       <c r="F93">
         <v>54</v>
       </c>
+      <c r="G93">
+        <v>0</v>
+      </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94">
@@ -10676,6 +10933,9 @@
       <c r="F94">
         <v>56</v>
       </c>
+      <c r="G94">
+        <v>0</v>
+      </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95">
@@ -10690,6 +10950,12 @@
       <c r="E95">
         <v>19</v>
       </c>
+      <c r="F95">
+        <v>0</v>
+      </c>
+      <c r="G95">
+        <v>0</v>
+      </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96">
@@ -10704,6 +10970,12 @@
       <c r="E96">
         <v>54</v>
       </c>
+      <c r="F96">
+        <v>0</v>
+      </c>
+      <c r="G96">
+        <v>0</v>
+      </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97">
@@ -10721,6 +10993,9 @@
       <c r="F97">
         <v>25</v>
       </c>
+      <c r="G97">
+        <v>0</v>
+      </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98">
@@ -10755,6 +11030,12 @@
       <c r="E99">
         <v>85</v>
       </c>
+      <c r="F99">
+        <v>0</v>
+      </c>
+      <c r="G99">
+        <v>0</v>
+      </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100">
@@ -10769,6 +11050,12 @@
       <c r="E100">
         <v>47</v>
       </c>
+      <c r="F100">
+        <v>0</v>
+      </c>
+      <c r="G100">
+        <v>0</v>
+      </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101">
@@ -10785,6 +11072,9 @@
       </c>
       <c r="F101">
         <v>58</v>
+      </c>
+      <c r="G101">
+        <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>